<commit_message>
Adds burn parameter to Problem 7 and updates pdf report
</commit_message>
<xml_diff>
--- a/lista1/data.xlsx
+++ b/lista1/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="14360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -507,7 +507,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:G1"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -552,9 +552,8 @@
       <c r="B2" s="13">
         <v>208256</v>
       </c>
-      <c r="C2" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E2:E13)</f>
-        <v>3327.6249592499994</v>
+      <c r="C2">
+        <v>4353.92</v>
       </c>
       <c r="D2" s="15">
         <v>156430949</v>
@@ -577,9 +576,8 @@
       <c r="B3" s="13">
         <v>450533.1</v>
       </c>
-      <c r="C3" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E14:E25)</f>
-        <v>3911.3916625833335</v>
+      <c r="C3">
+        <v>4299</v>
       </c>
       <c r="D3" s="15">
         <v>158874963</v>
@@ -602,9 +600,8 @@
       <c r="B4" s="13">
         <v>557896.5</v>
       </c>
-      <c r="C4" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E26:E37)</f>
-        <v>5922.4083250833328</v>
+      <c r="C4">
+        <v>7039.94</v>
       </c>
       <c r="D4" s="15">
         <v>161323169</v>
@@ -627,9 +624,8 @@
       <c r="B5" s="13">
         <v>622871.80000000005</v>
       </c>
-      <c r="C5" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E38:E49)</f>
-        <v>10299.033365833333</v>
+      <c r="C5">
+        <v>10196.5</v>
       </c>
       <c r="D5" s="15">
         <v>163779827</v>
@@ -652,9 +648,8 @@
       <c r="B6" s="13">
         <v>644033.1</v>
       </c>
-      <c r="C6" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E50:E61)</f>
-        <v>9139.5</v>
+      <c r="C6">
+        <v>6784.3</v>
       </c>
       <c r="D6" s="15">
         <v>166252088</v>
@@ -677,9 +672,8 @@
       <c r="B7" s="13">
         <v>704738.4</v>
       </c>
-      <c r="C7" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E62:E73)</f>
-        <v>11377.583333333334</v>
+      <c r="C7">
+        <v>17091.599999999999</v>
       </c>
       <c r="D7" s="15">
         <v>168753552</v>
@@ -702,9 +696,8 @@
       <c r="B8" s="13">
         <v>775853.7</v>
       </c>
-      <c r="C8" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E74:E85)</f>
-        <v>16019.5</v>
+      <c r="C8">
+        <v>15259.2</v>
       </c>
       <c r="D8" s="15">
         <v>171279882</v>
@@ -727,9 +720,8 @@
       <c r="B9" s="13">
         <v>843887.7</v>
       </c>
-      <c r="C9" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E86:E97)</f>
-        <v>13936.333333333334</v>
+      <c r="C9">
+        <v>13577.5</v>
       </c>
       <c r="D9" s="15">
         <v>172385826</v>
@@ -752,9 +744,8 @@
       <c r="B10" s="13">
         <v>923575.5</v>
       </c>
-      <c r="C10" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E98:E109)</f>
-        <v>11483.916666666666</v>
+      <c r="C10">
+        <v>11268.4</v>
       </c>
       <c r="D10" s="15">
         <v>174632960</v>
@@ -777,9 +768,8 @@
       <c r="B11" s="13">
         <v>1063141.6000000001</v>
       </c>
-      <c r="C11" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E110:E121)</f>
-        <v>14717.25</v>
+      <c r="C11">
+        <v>22236.3</v>
       </c>
       <c r="D11" s="15">
         <v>176871437</v>
@@ -802,9 +792,8 @@
       <c r="B12" s="13">
         <v>1179849.8999999999</v>
       </c>
-      <c r="C12" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E122:E133)</f>
-        <v>22400.833333333332</v>
+      <c r="C12">
+        <v>26196.25</v>
       </c>
       <c r="D12" s="15">
         <v>181581024</v>
@@ -827,9 +816,8 @@
       <c r="B13" s="13">
         <v>1312672</v>
       </c>
-      <c r="C13" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E134:E145)</f>
-        <v>27953.416666666668</v>
+      <c r="C13">
+        <v>33455.94</v>
       </c>
       <c r="D13" s="15">
         <v>184184264</v>
@@ -852,9 +840,8 @@
       <c r="B14" s="13">
         <v>1456420.4</v>
       </c>
-      <c r="C14" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E146:E157)</f>
-        <v>38658</v>
+      <c r="C14">
+        <v>44473.71</v>
       </c>
       <c r="D14" s="15">
         <v>186770562</v>
@@ -877,9 +864,8 @@
       <c r="B15" s="13">
         <v>1628509.9</v>
       </c>
-      <c r="C15" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E158:E169)</f>
-        <v>54287.5</v>
+      <c r="C15">
+        <v>63886.1</v>
       </c>
       <c r="D15" s="15">
         <v>183989711</v>
@@ -902,9 +888,8 @@
       <c r="B16" s="13">
         <v>1857401.3</v>
       </c>
-      <c r="C16" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E170:E181)</f>
-        <v>55462.916666666664</v>
+      <c r="C16">
+        <v>37550.31</v>
       </c>
       <c r="D16" s="15">
         <v>189612814</v>
@@ -927,9 +912,8 @@
       <c r="B17" s="13">
         <v>2063996.2</v>
       </c>
-      <c r="C17" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E182:E1193)</f>
-        <v>57805.930555555555</v>
+      <c r="C17">
+        <v>68588.41</v>
       </c>
       <c r="D17" s="15">
         <v>191480630</v>
@@ -952,9 +936,8 @@
       <c r="B18" s="13">
         <v>2341155</v>
       </c>
-      <c r="C18" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E194:E205)</f>
-        <v>66963.583333333328</v>
+      <c r="C18">
+        <v>69304.81</v>
       </c>
       <c r="D18" s="15">
         <v>190747855</v>
@@ -977,9 +960,8 @@
       <c r="B19" s="13">
         <v>2637009</v>
       </c>
-      <c r="C19" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E206:E217)</f>
-        <v>61275.916666666664</v>
+      <c r="C19">
+        <v>56754.080000000002</v>
       </c>
       <c r="D19" s="15">
         <v>192379287</v>
@@ -1002,9 +984,8 @@
       <c r="B20" s="13">
         <v>2908410.2</v>
       </c>
-      <c r="C20" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E218:E229)</f>
-        <v>59324.083333333336</v>
+      <c r="C20">
+        <v>60952.08</v>
       </c>
       <c r="D20" s="15">
         <v>193946886</v>
@@ -1027,9 +1008,8 @@
       <c r="B21" s="13">
         <v>3200737</v>
       </c>
-      <c r="C21" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E230:E241)</f>
-        <v>53269.583333333336</v>
+      <c r="C21">
+        <v>51507.16</v>
       </c>
       <c r="D21" s="15">
         <v>201032714</v>
@@ -1052,9 +1032,8 @@
       <c r="B22" s="13">
         <v>3449806.9</v>
       </c>
-      <c r="C22" s="13">
-        <f>AVERAGE('BVSP (Yahoo Finance)'!E242:E253)</f>
-        <v>52642.916666666664</v>
+      <c r="C22">
+        <v>50007.41</v>
       </c>
       <c r="D22" s="15">
         <v>202768562</v>

</xml_diff>